<commit_message>
cap nhat ho so simple
</commit_message>
<xml_diff>
--- a/web/dem_xe.xlsx
+++ b/web/dem_xe.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\CV\2024\TruongLai\pmDaoTao\quanlydaotao\web\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3375AF2D-C977-46D6-A852-FDCEB1684269}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B6A02FB8-FD2B-4353-9368-ED6E64393826}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="10725" yWindow="90" windowWidth="18045" windowHeight="15330" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="32">
   <si>
     <t>STT</t>
   </si>
@@ -36,9 +36,6 @@
     <t>Tổng số giờ</t>
   </si>
   <si>
-    <t>84A-142.58</t>
-  </si>
-  <si>
     <t>84A-142.59</t>
   </si>
   <si>
@@ -54,9 +51,6 @@
     <t>84A-147.25</t>
   </si>
   <si>
-    <t>2025-11-18 07:00:00</t>
-  </si>
-  <si>
     <t>Giờ đi</t>
   </si>
   <si>
@@ -118,6 +112,15 @@
   </si>
   <si>
     <t>Bảng giờ xe ra vào</t>
+  </si>
+  <si>
+    <t>84A-245.53</t>
+  </si>
+  <si>
+    <t>2025-11-25 07:00:00</t>
+  </si>
+  <si>
+    <t>2025-11-25 14:00:00</t>
   </si>
 </sst>
 </file>
@@ -201,14 +204,14 @@
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -492,7 +495,7 @@
   <dimension ref="A1:E13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J9" sqref="J9"/>
+      <selection activeCell="M26" sqref="M26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -501,40 +504,40 @@
     <col min="2" max="2" width="14.7109375" customWidth="1"/>
     <col min="3" max="3" width="18.28515625" style="5" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="18.28515625" style="5" customWidth="1"/>
-    <col min="5" max="5" width="19" customWidth="1"/>
+    <col min="5" max="5" width="18" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="21" x14ac:dyDescent="0.35">
-      <c r="A1" s="6" t="s">
-        <v>30</v>
-      </c>
-      <c r="B1" s="6"/>
-      <c r="C1" s="6"/>
-      <c r="D1" s="6"/>
-      <c r="E1" s="6"/>
+      <c r="A1" s="9" t="s">
+        <v>28</v>
+      </c>
+      <c r="B1" s="9"/>
+      <c r="C1" s="9"/>
+      <c r="D1" s="9"/>
+      <c r="E1" s="9"/>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="D2" s="5" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="E2" s="5" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" s="7" t="s">
+      <c r="A3" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="B3" s="8" t="s">
+      <c r="B3" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="9" t="s">
-        <v>10</v>
-      </c>
-      <c r="D3" s="9" t="s">
-        <v>11</v>
-      </c>
-      <c r="E3" s="8" t="s">
+      <c r="C3" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="D3" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="E3" s="7" t="s">
         <v>2</v>
       </c>
     </row>
@@ -543,16 +546,16 @@
         <v>1</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>3</v>
+        <v>29</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>9</v>
+        <v>30</v>
       </c>
       <c r="D4" s="4" t="s">
-        <v>12</v>
+        <v>31</v>
       </c>
       <c r="E4" s="1">
-        <v>2</v>
+        <v>7</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
@@ -560,13 +563,13 @@
         <v>2</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="D5" s="4" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="E5" s="1">
         <v>0.25</v>
@@ -577,13 +580,13 @@
         <v>3</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="D6" s="4" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="E6" s="1">
         <v>8.3000000000000004E-2</v>
@@ -594,13 +597,13 @@
         <v>4</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C7" s="4" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="D7" s="4" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="E7" s="1">
         <v>0.75</v>
@@ -611,13 +614,13 @@
         <v>5</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C8" s="4" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="D8" s="4" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="E8" s="1">
         <v>2</v>
@@ -628,13 +631,13 @@
         <v>6</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C9" s="4" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="D9" s="4" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="E9" s="1">
         <v>1</v>
@@ -645,13 +648,13 @@
         <v>7</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C10" s="4" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="D10" s="4" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="E10" s="1">
         <v>0.25</v>
@@ -662,13 +665,13 @@
         <v>8</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C11" s="4" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="D11" s="4" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="E11" s="1">
         <v>2</v>
@@ -679,13 +682,13 @@
         <v>9</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C12" s="4" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="D12" s="4" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="E12" s="1">
         <v>0.75</v>
@@ -696,13 +699,13 @@
         <v>10</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C13" s="4" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="D13" s="4" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="E13" s="1">
         <v>1</v>

</xml_diff>